<commit_message>
Adicionado resultados sem o wavelets
</commit_message>
<xml_diff>
--- a/resultados/resultados com wavelet.xlsx
+++ b/resultados/resultados com wavelet.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="LRC" sheetId="2" r:id="rId1"/>
+    <sheet name="LRC - Wavelet" sheetId="1" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
-  <si>
-    <t>LRC - Wavelet (100 holdouts experimento)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t>Taxa de acerto</t>
   </si>
@@ -58,6 +55,36 @@
   </si>
   <si>
     <t>YaleB - Waveletfaces lvl3</t>
+  </si>
+  <si>
+    <t>ARFaces</t>
+  </si>
+  <si>
+    <t>Taxa de Acerto</t>
+  </si>
+  <si>
+    <t>Desvio Padrao</t>
+  </si>
+  <si>
+    <t>YaleB</t>
+  </si>
+  <si>
+    <t>Gtech</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>GTech - Waveletfaces lvl3</t>
+  </si>
+  <si>
+    <t>EssexFaces</t>
+  </si>
+  <si>
+    <t>LRC - 100 holdout experimento (50% treino - 50% teste)</t>
+  </si>
+  <si>
+    <t>LRC - Wavelet - 100 holdouts experimento (50% treino - 50% teste)</t>
   </si>
 </sst>
 </file>
@@ -103,11 +130,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +429,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>0.81005384615384601</v>
+      </c>
+      <c r="C3">
+        <v>0.929095394736842</v>
+      </c>
+      <c r="D3">
+        <v>0.77851428571428605</v>
+      </c>
+      <c r="E3">
+        <v>0.9587</v>
+      </c>
+      <c r="F3">
+        <v>0.92076388888888805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1.21941415948623E-2</v>
+      </c>
+      <c r="C4">
+        <v>7.7335851447940598E-3</v>
+      </c>
+      <c r="D4">
+        <v>1.9583290240613602E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.6199825413699499E-2</v>
+      </c>
+      <c r="F4">
+        <v>9.1967057889631998E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -418,55 +525,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="B4">
         <v>0.85646923076922998</v>
@@ -491,8 +598,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+      <c r="A5" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B5">
         <v>1.1669596701664E-2</v>
@@ -517,43 +624,43 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="2" t="s">
-        <v>1</v>
+      <c r="A9" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B9">
         <v>0.88716666666666599</v>
@@ -567,7 +674,7 @@
       <c r="E9">
         <v>0.87961111111111101</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0.90175000000000005</v>
       </c>
       <c r="G9">
@@ -578,8 +685,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
+      <c r="A10" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B10">
         <v>1.11625792092676E-2</v>
@@ -599,48 +706,48 @@
       <c r="G10">
         <v>1.14263666303588E-2</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>1.10364555437884E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="2" t="s">
-        <v>1</v>
+      <c r="A14" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B14">
         <v>0.96689999999999998</v>
@@ -665,8 +772,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="2" t="s">
-        <v>2</v>
+      <c r="A15" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B15">
         <v>1.6063966521633499E-2</v>
@@ -691,43 +798,43 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
-        <v>1</v>
+      <c r="A19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B19">
         <v>0.953519736842105</v>
@@ -752,8 +859,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
-        <v>2</v>
+      <c r="A20" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B20">
         <v>5.4128354620184699E-3</v>
@@ -778,43 +885,43 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="2" t="s">
-        <v>1</v>
+      <c r="A24" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B24">
         <v>0.79291428571428602</v>
@@ -839,8 +946,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="2" t="s">
-        <v>2</v>
+      <c r="A25" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B25">
         <v>1.72130729161586E-2</v>
@@ -866,27 +973,15 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 

</xml_diff>